<commit_message>
cleaned up code and used updated annotation files
</commit_message>
<xml_diff>
--- a/patient_table.xlsx
+++ b/patient_table.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/ICU_EEG_old/ICU_EEG_MATLAB/Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/ICU_EEG_old/ICU_EEG_MATLAB/Final/ICU_EEG_Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF56FF5-8646-E648-BC14-AFB5EC96F107}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{535BD64B-5C7F-1643-AFB8-3C84659D9F8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="1100" windowWidth="26040" windowHeight="14940" xr2:uid="{00CE0698-3822-F844-BBD9-C1AB2AB6089E}"/>
+    <workbookView xWindow="3340" yWindow="3180" windowWidth="26040" windowHeight="14580" xr2:uid="{00CE0698-3822-F844-BBD9-C1AB2AB6089E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="patient_table_new" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="122">
   <si>
     <t>portal_id</t>
   </si>
@@ -303,56 +303,101 @@
     <t>CNT782</t>
   </si>
   <si>
-    <t>ICUDataRedux_0007</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0008</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0009</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0010</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0011</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0012</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0013</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0014</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0015</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0016</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0017</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0018</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0019</t>
-  </si>
-  <si>
-    <t>ICUDataRedux_0020</t>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Test_set</t>
+  </si>
+  <si>
+    <t>CNT929</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0027</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0028</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0033</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0036</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0040</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0042</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0045</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0049</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0050</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0023</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0026</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0029</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0030</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0034</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0035</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0043</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0044</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0047</t>
+  </si>
+  <si>
+    <t>ICUDataRedux_0048</t>
+  </si>
+  <si>
+    <t>sz_num</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>num_artifact</t>
+  </si>
+  <si>
+    <t>mean_sz_len</t>
+  </si>
+  <si>
+    <t>record_len</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -367,11 +412,17 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -394,10 +445,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,20 +764,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31674987-35E1-8E4F-9644-E80B02F4F39C}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -738,8 +792,29 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -752,8 +827,29 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>100.5</v>
+      </c>
+      <c r="J2">
+        <v>30000</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -766,8 +862,29 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>49</v>
+      </c>
+      <c r="I3">
+        <v>110.18</v>
+      </c>
+      <c r="J3">
+        <v>31855</v>
+      </c>
+      <c r="K3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -780,8 +897,29 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <v>22.135999999999999</v>
+      </c>
+      <c r="J4">
+        <v>23500</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -794,8 +932,29 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>20.8</v>
+      </c>
+      <c r="J5">
+        <v>30170</v>
+      </c>
+      <c r="K5">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -808,8 +967,29 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <v>74.179000000000002</v>
+      </c>
+      <c r="J6">
+        <v>14995</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -822,8 +1002,29 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>139</v>
+      </c>
+      <c r="J7">
+        <v>7000</v>
+      </c>
+      <c r="K7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -836,8 +1037,29 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>224.2</v>
+      </c>
+      <c r="J8">
+        <v>37000</v>
+      </c>
+      <c r="K8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -850,8 +1072,29 @@
       <c r="D9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>139</v>
+      </c>
+      <c r="J9">
+        <v>32975</v>
+      </c>
+      <c r="K9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -864,8 +1107,29 @@
       <c r="D10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>29.75</v>
+      </c>
+      <c r="J10">
+        <v>10000</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -878,8 +1142,29 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="I11">
+        <v>12.909000000000001</v>
+      </c>
+      <c r="J11">
+        <v>2955</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -892,8 +1177,29 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>21.582999999999998</v>
+      </c>
+      <c r="J12">
+        <v>5000</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -906,8 +1212,29 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>68</v>
+      </c>
+      <c r="J13">
+        <v>20000</v>
+      </c>
+      <c r="K13">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -920,8 +1247,29 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <v>130.55000000000001</v>
+      </c>
+      <c r="J14">
+        <v>10000</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -934,8 +1282,29 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>104.6</v>
+      </c>
+      <c r="J15">
+        <v>16000</v>
+      </c>
+      <c r="K15">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -948,8 +1317,29 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>1260.5</v>
+      </c>
+      <c r="J16">
+        <v>10000</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -962,8 +1352,29 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>54</v>
+      </c>
+      <c r="F17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>134.69999999999999</v>
+      </c>
+      <c r="J17">
+        <v>2800</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -976,8 +1387,29 @@
       <c r="D18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>42</v>
+      </c>
+      <c r="J18">
+        <v>10000</v>
+      </c>
+      <c r="K18">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -990,8 +1422,29 @@
       <c r="D19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>147</v>
+      </c>
+      <c r="J19">
+        <v>5000</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1004,8 +1457,29 @@
       <c r="D20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>52</v>
+      </c>
+      <c r="F20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>22</v>
+      </c>
+      <c r="I20">
+        <v>266</v>
+      </c>
+      <c r="J20">
+        <v>15085</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1018,8 +1492,29 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>16</v>
+      </c>
+      <c r="I21">
+        <v>67.125</v>
+      </c>
+      <c r="J21">
+        <v>9570</v>
+      </c>
+      <c r="K21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1032,8 +1527,26 @@
       <c r="D22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <v>95.6</v>
+      </c>
+      <c r="J22">
+        <v>10000</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1046,8 +1559,29 @@
       <c r="D23" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>265.60000000000002</v>
+      </c>
+      <c r="J23">
+        <v>8000</v>
+      </c>
+      <c r="K23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1060,8 +1594,29 @@
       <c r="D24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>18</v>
+      </c>
+      <c r="I24">
+        <v>94.221999999999994</v>
+      </c>
+      <c r="J24">
+        <v>5000</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1074,8 +1629,26 @@
       <c r="D25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>315.33</v>
+      </c>
+      <c r="J25">
+        <v>2000</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1088,8 +1661,23 @@
       <c r="D26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>96</v>
+      </c>
+      <c r="J26">
+        <v>5000</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1102,8 +1690,23 @@
       <c r="D27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <v>10000</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1116,8 +1719,23 @@
       <c r="D28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>582</v>
+      </c>
+      <c r="J28">
+        <v>5000</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1130,8 +1748,29 @@
       <c r="D29" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29">
+        <v>10000</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1144,8 +1783,29 @@
       <c r="D30" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>22</v>
+      </c>
+      <c r="F30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>121</v>
+      </c>
+      <c r="J30">
+        <v>10000</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1158,8 +1818,29 @@
       <c r="D31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>121</v>
+      </c>
+      <c r="J31">
+        <v>10000</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1172,8 +1853,29 @@
       <c r="D32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>116</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>121</v>
+      </c>
+      <c r="J32">
+        <v>10000</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -1186,8 +1888,29 @@
       <c r="D33" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>74</v>
+      </c>
+      <c r="F33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>121</v>
+      </c>
+      <c r="J33">
+        <v>10000</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1200,8 +1923,29 @@
       <c r="D34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>71</v>
+      </c>
+      <c r="F34" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>121</v>
+      </c>
+      <c r="J34">
+        <v>10000</v>
+      </c>
+      <c r="K34">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1214,8 +1958,29 @@
       <c r="D35" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>69</v>
+      </c>
+      <c r="F35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>121</v>
+      </c>
+      <c r="J35">
+        <v>10000</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -1228,8 +1993,29 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>84</v>
+      </c>
+      <c r="F36" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36">
+        <v>10000</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1242,8 +2028,29 @@
       <c r="D37" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>24</v>
+      </c>
+      <c r="F37" t="s">
+        <v>116</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>121</v>
+      </c>
+      <c r="J37">
+        <v>10000</v>
+      </c>
+      <c r="K37">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1256,8 +2063,29 @@
       <c r="D38" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>64</v>
+      </c>
+      <c r="F38" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>121</v>
+      </c>
+      <c r="J38">
+        <v>10000</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1270,8 +2098,29 @@
       <c r="D39" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>61</v>
+      </c>
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>121</v>
+      </c>
+      <c r="J39">
+        <v>10000</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1284,8 +2133,29 @@
       <c r="D40" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>60</v>
+      </c>
+      <c r="F40" t="s">
+        <v>116</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>121</v>
+      </c>
+      <c r="J40">
+        <v>10000</v>
+      </c>
+      <c r="K40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1298,8 +2168,29 @@
       <c r="D41" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>64</v>
+      </c>
+      <c r="F41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>121</v>
+      </c>
+      <c r="J41">
+        <v>10000</v>
+      </c>
+      <c r="K41">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1312,8 +2203,29 @@
       <c r="D42" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>65</v>
+      </c>
+      <c r="F42" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>121</v>
+      </c>
+      <c r="J42">
+        <v>10000</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1326,8 +2238,29 @@
       <c r="D43" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>67</v>
+      </c>
+      <c r="F43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>121</v>
+      </c>
+      <c r="J43">
+        <v>10000</v>
+      </c>
+      <c r="K43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1340,8 +2273,29 @@
       <c r="D44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>60</v>
+      </c>
+      <c r="F44" t="s">
+        <v>116</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>121</v>
+      </c>
+      <c r="J44">
+        <v>10000</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1354,8 +2308,29 @@
       <c r="D45" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>67</v>
+      </c>
+      <c r="F45" t="s">
+        <v>116</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>121</v>
+      </c>
+      <c r="J45">
+        <v>10000</v>
+      </c>
+      <c r="K45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -1368,8 +2343,29 @@
       <c r="D46" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>63</v>
+      </c>
+      <c r="F46" t="s">
+        <v>116</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>121</v>
+      </c>
+      <c r="J46">
+        <v>10000</v>
+      </c>
+      <c r="K46">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -1382,8 +2378,29 @@
       <c r="D47" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>121</v>
+      </c>
+      <c r="J47">
+        <v>10000</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -1396,8 +2413,29 @@
       <c r="D48" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>53</v>
+      </c>
+      <c r="F48" t="s">
+        <v>116</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>121</v>
+      </c>
+      <c r="J48">
+        <v>10000</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -1410,8 +2448,29 @@
       <c r="D49" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>75</v>
+      </c>
+      <c r="F49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>121</v>
+      </c>
+      <c r="J49">
+        <v>10000</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -1424,8 +2483,29 @@
       <c r="D50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>55</v>
+      </c>
+      <c r="F50" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>121</v>
+      </c>
+      <c r="J50">
+        <v>10000</v>
+      </c>
+      <c r="K50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -1438,8 +2518,29 @@
       <c r="D51" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>22</v>
+      </c>
+      <c r="F51" t="s">
+        <v>116</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>121</v>
+      </c>
+      <c r="J51">
+        <v>10000</v>
+      </c>
+      <c r="K51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -1452,8 +2553,29 @@
       <c r="D52" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>22</v>
+      </c>
+      <c r="F52" t="s">
+        <v>116</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>121</v>
+      </c>
+      <c r="J52">
+        <v>10000</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1466,8 +2588,29 @@
       <c r="D53" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>86</v>
+      </c>
+      <c r="F53" t="s">
+        <v>116</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>121</v>
+      </c>
+      <c r="J53">
+        <v>10000</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -1480,8 +2623,29 @@
       <c r="D54" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>67</v>
+      </c>
+      <c r="F54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>121</v>
+      </c>
+      <c r="J54">
+        <v>10000</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -1494,8 +2658,29 @@
       <c r="D55" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>19</v>
+      </c>
+      <c r="F55" t="s">
+        <v>117</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>121</v>
+      </c>
+      <c r="J55">
+        <v>10000</v>
+      </c>
+      <c r="K55">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -1508,8 +2693,29 @@
       <c r="D56" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>61</v>
+      </c>
+      <c r="F56" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>121</v>
+      </c>
+      <c r="J56">
+        <v>10000</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -1522,8 +2728,29 @@
       <c r="D57" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>45</v>
+      </c>
+      <c r="F57" t="s">
+        <v>117</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>121</v>
+      </c>
+      <c r="J57">
+        <v>10000</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -1536,8 +2763,29 @@
       <c r="D58" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>75</v>
+      </c>
+      <c r="F58" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>121</v>
+      </c>
+      <c r="J58">
+        <v>10000</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -1550,8 +2798,29 @@
       <c r="D59" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>72</v>
+      </c>
+      <c r="F59" t="s">
+        <v>117</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>121</v>
+      </c>
+      <c r="J59">
+        <v>10000</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -1564,8 +2833,29 @@
       <c r="D60" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>53</v>
+      </c>
+      <c r="F60" t="s">
+        <v>116</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>121</v>
+      </c>
+      <c r="J60">
+        <v>10000</v>
+      </c>
+      <c r="K60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -1578,8 +2868,29 @@
       <c r="D61" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>52</v>
+      </c>
+      <c r="F61" t="s">
+        <v>117</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>121</v>
+      </c>
+      <c r="J61">
+        <v>10000</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -1592,8 +2903,29 @@
       <c r="D62" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>68</v>
+      </c>
+      <c r="F62" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62" t="s">
+        <v>121</v>
+      </c>
+      <c r="J62">
+        <v>10000</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -1606,8 +2938,29 @@
       <c r="D63" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>38</v>
+      </c>
+      <c r="F63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>121</v>
+      </c>
+      <c r="J63">
+        <v>10000</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -1620,8 +2973,29 @@
       <c r="D64" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>60</v>
+      </c>
+      <c r="F64" t="s">
+        <v>116</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>121</v>
+      </c>
+      <c r="J64">
+        <v>10000</v>
+      </c>
+      <c r="K64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>78</v>
       </c>
@@ -1634,8 +3008,29 @@
       <c r="D65" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>54</v>
+      </c>
+      <c r="F65" t="s">
+        <v>116</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>121</v>
+      </c>
+      <c r="J65">
+        <v>10000</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -1648,8 +3043,29 @@
       <c r="D66" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>64</v>
+      </c>
+      <c r="F66" t="s">
+        <v>116</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>121</v>
+      </c>
+      <c r="J66">
+        <v>10000</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -1662,8 +3078,29 @@
       <c r="D67" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>44</v>
+      </c>
+      <c r="F67" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="s">
+        <v>121</v>
+      </c>
+      <c r="J67">
+        <v>10000</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -1676,8 +3113,29 @@
       <c r="D68" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>53</v>
+      </c>
+      <c r="F68" t="s">
+        <v>116</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
+        <v>121</v>
+      </c>
+      <c r="J68">
+        <v>10000</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -1690,8 +3148,29 @@
       <c r="D69" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>62</v>
+      </c>
+      <c r="F69" t="s">
+        <v>116</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>121</v>
+      </c>
+      <c r="J69">
+        <v>10000</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -1704,8 +3183,29 @@
       <c r="D70" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>74</v>
+      </c>
+      <c r="F70" t="s">
+        <v>117</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>121</v>
+      </c>
+      <c r="J70">
+        <v>10000</v>
+      </c>
+      <c r="K70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -1718,8 +3218,29 @@
       <c r="D71" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>20</v>
+      </c>
+      <c r="F71" t="s">
+        <v>117</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
+        <v>121</v>
+      </c>
+      <c r="J71">
+        <v>10000</v>
+      </c>
+      <c r="K71">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -1732,8 +3253,29 @@
       <c r="D72" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>81</v>
+      </c>
+      <c r="F72" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J72">
+        <v>10000</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -1746,8 +3288,29 @@
       <c r="D73" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>81</v>
+      </c>
+      <c r="F73" t="s">
+        <v>116</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73" t="s">
+        <v>121</v>
+      </c>
+      <c r="J73">
+        <v>10000</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -1760,8 +3323,29 @@
       <c r="D74" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>44</v>
+      </c>
+      <c r="F74" t="s">
+        <v>116</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74" t="s">
+        <v>121</v>
+      </c>
+      <c r="J74">
+        <v>10000</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -1774,8 +3358,29 @@
       <c r="D75" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>67</v>
+      </c>
+      <c r="F75" t="s">
+        <v>116</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75" t="s">
+        <v>121</v>
+      </c>
+      <c r="J75">
+        <v>10000</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>89</v>
       </c>
@@ -1788,8 +3393,29 @@
       <c r="D76" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>60</v>
+      </c>
+      <c r="F76" t="s">
+        <v>117</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76" t="s">
+        <v>121</v>
+      </c>
+      <c r="J76">
+        <v>10000</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>90</v>
       </c>
@@ -1802,8 +3428,29 @@
       <c r="D77" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>66</v>
+      </c>
+      <c r="F77" t="s">
+        <v>117</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" t="s">
+        <v>121</v>
+      </c>
+      <c r="J77">
+        <v>10000</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -1816,204 +3463,677 @@
       <c r="D78" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>92</v>
+      <c r="E78">
+        <v>47</v>
+      </c>
+      <c r="F78" t="s">
+        <v>117</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78" t="s">
+        <v>121</v>
+      </c>
+      <c r="J78">
+        <v>10000</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B79" s="2">
+        <v>113</v>
+      </c>
+      <c r="C79" s="2">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>132</v>
+      </c>
+      <c r="J79">
+        <v>20000</v>
+      </c>
+      <c r="K79">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="2">
+        <v>116</v>
+      </c>
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80">
+        <v>74</v>
+      </c>
+      <c r="F80" t="s">
+        <v>116</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>909</v>
+      </c>
+      <c r="J80">
+        <v>10000</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81" s="2">
+        <v>117</v>
+      </c>
+      <c r="C81" s="2">
+        <v>1</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81">
+        <v>68</v>
+      </c>
+      <c r="F81" t="s">
+        <v>117</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>3</v>
+      </c>
+      <c r="I81">
+        <v>310</v>
+      </c>
+      <c r="J81">
+        <v>10000</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" s="2">
+        <v>118</v>
+      </c>
+      <c r="C82" s="2">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82">
+        <v>79</v>
+      </c>
+      <c r="F82" t="s">
+        <v>117</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>6</v>
+      </c>
+      <c r="I82">
+        <v>62.5</v>
+      </c>
+      <c r="J82">
+        <v>5000</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" s="2">
+        <v>119</v>
+      </c>
+      <c r="C83" s="2">
+        <v>1</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83">
+        <v>86</v>
+      </c>
+      <c r="F83" t="s">
+        <v>116</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>193</v>
+      </c>
+      <c r="J83">
+        <v>2000</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B84" s="2">
+        <v>120</v>
+      </c>
+      <c r="C84" s="2">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84">
+        <v>74</v>
+      </c>
+      <c r="F84" t="s">
+        <v>116</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>5000</v>
+      </c>
+      <c r="J84">
+        <v>5000</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="2">
+        <v>121</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
+        <v>117</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>2</v>
+      </c>
+      <c r="I85">
+        <v>52.5</v>
+      </c>
+      <c r="J85">
+        <v>13000</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="2">
+        <v>122</v>
+      </c>
+      <c r="C86" s="2">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86">
+        <v>60</v>
+      </c>
+      <c r="F86" t="s">
+        <v>117</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
         <v>95</v>
       </c>
-      <c r="C79" s="2">
-        <v>3</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B80" s="2">
-        <v>96</v>
-      </c>
-      <c r="C80" s="2">
-        <v>3</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B81" s="2">
-        <v>97</v>
-      </c>
-      <c r="C81" s="2">
-        <v>3</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" s="2">
-        <v>98</v>
-      </c>
-      <c r="C82" s="2">
-        <v>3</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B83" s="2">
-        <v>99</v>
-      </c>
-      <c r="C83" s="2">
-        <v>3</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B84" s="2">
-        <v>100</v>
-      </c>
-      <c r="C84" s="2">
-        <v>3</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B85" s="2">
-        <v>101</v>
-      </c>
-      <c r="C85" s="2">
-        <v>3</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B86" s="2">
-        <v>102</v>
-      </c>
-      <c r="C86" s="2">
-        <v>3</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>101</v>
+      <c r="J86">
+        <v>7000</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B87" s="2">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C87" s="2">
-        <v>3</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>102</v>
+        <v>1</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87">
+        <v>16</v>
+      </c>
+      <c r="F87" t="s">
+        <v>117</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>9</v>
+      </c>
+      <c r="I87">
+        <v>38.889000000000003</v>
+      </c>
+      <c r="J87">
+        <v>10000</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B88" s="2">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C88" s="2">
-        <v>3</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>103</v>
+        <v>1</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88">
+        <v>21</v>
+      </c>
+      <c r="F88" t="s">
+        <v>116</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>2</v>
+      </c>
+      <c r="I88">
+        <v>63</v>
+      </c>
+      <c r="J88">
+        <v>5000</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B89" s="2">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="C89" s="2">
-        <v>3</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>104</v>
+        <v>2</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89">
+        <v>51</v>
+      </c>
+      <c r="F89" t="s">
+        <v>116</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89" t="s">
+        <v>121</v>
+      </c>
+      <c r="J89">
+        <v>10000</v>
+      </c>
+      <c r="K89">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B90" s="2">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="C90" s="2">
-        <v>3</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>105</v>
+        <v>2</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90">
+        <v>74</v>
+      </c>
+      <c r="F90" t="s">
+        <v>116</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>121</v>
+      </c>
+      <c r="J90">
+        <v>10000</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="B91" s="2">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="C91" s="2">
-        <v>3</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>106</v>
+        <v>2</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91">
+        <v>73</v>
+      </c>
+      <c r="F91" t="s">
+        <v>117</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91" t="s">
+        <v>121</v>
+      </c>
+      <c r="J91">
+        <v>10000</v>
+      </c>
+      <c r="K91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B92" s="2">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C92" s="2">
-        <v>3</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>93</v>
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>43</v>
+      </c>
+      <c r="F92" t="s">
+        <v>117</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>121</v>
+      </c>
+      <c r="J92">
+        <v>10000</v>
+      </c>
+      <c r="K92">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B93" s="2">
+        <v>129</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <v>49</v>
+      </c>
+      <c r="F93" t="s">
+        <v>116</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93" t="s">
+        <v>121</v>
+      </c>
+      <c r="J93">
+        <v>10000</v>
+      </c>
+      <c r="K93">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B94" s="2">
+        <v>130</v>
+      </c>
+      <c r="C94" s="2">
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <v>30</v>
+      </c>
+      <c r="F94" t="s">
+        <v>117</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94" t="s">
+        <v>121</v>
+      </c>
+      <c r="J94">
+        <v>10000</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" s="2">
+        <v>131</v>
+      </c>
+      <c r="C95" s="2">
+        <v>2</v>
+      </c>
+      <c r="E95">
+        <v>38</v>
+      </c>
+      <c r="F95" t="s">
+        <v>116</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>121</v>
+      </c>
+      <c r="J95">
+        <v>10000</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B96" s="2">
+        <v>132</v>
+      </c>
+      <c r="C96" s="2">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <v>64</v>
+      </c>
+      <c r="F96" t="s">
+        <v>117</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96" t="s">
+        <v>121</v>
+      </c>
+      <c r="J96">
+        <v>10000</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B97" s="2">
+        <v>133</v>
+      </c>
+      <c r="C97" s="2">
+        <v>2</v>
+      </c>
+      <c r="E97">
+        <v>58</v>
+      </c>
+      <c r="F97" t="s">
+        <v>116</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97" t="s">
+        <v>121</v>
+      </c>
+      <c r="J97">
+        <v>10000</v>
+      </c>
+      <c r="K97">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98" s="2">
+        <v>134</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2</v>
+      </c>
+      <c r="E98">
+        <v>60</v>
+      </c>
+      <c r="F98" t="s">
+        <v>116</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>121</v>
+      </c>
+      <c r="J98">
+        <v>10000</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>